<commit_message>
add dual nlm experiments
</commit_message>
<xml_diff>
--- a/data/output/pg_noisy/results/dual.xlsx
+++ b/data/output/pg_noisy/results/dual.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\GaussianExperiments\data\output\set12\moderate_noisy\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\GaussianExperiments\data\output\pg_noisy\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA65E54-579F-440B-8F67-CE347DBCDF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA877A6-F38A-4D93-AB4F-BB23F7EA701C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,40 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>06.png</t>
-  </si>
-  <si>
-    <t>01.png</t>
-  </si>
-  <si>
-    <t>03.png</t>
-  </si>
-  <si>
-    <t>10.png</t>
-  </si>
-  <si>
-    <t>05.png</t>
-  </si>
-  <si>
-    <t>09.png</t>
-  </si>
-  <si>
-    <t>11.png</t>
-  </si>
-  <si>
-    <t>02.png</t>
-  </si>
-  <si>
-    <t>07.png</t>
-  </si>
-  <si>
-    <t>04.png</t>
-  </si>
-  <si>
-    <t>08.png</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Imagem</t>
   </si>
@@ -65,6 +32,12 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>PSNR = 22.08 | SSIM = 0.4068 | Score = 31.38</t>
+  </si>
+  <si>
+    <t>PSNR = 22.78 | SSIM = 0.4333 | Score = 33.05</t>
   </si>
 </sst>
 </file>
@@ -434,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D12"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,174 +423,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>34.621974616093098</v>
-      </c>
-      <c r="C2">
-        <v>0.92839473297007802</v>
-      </c>
-      <c r="D2">
-        <v>63.730723956550499</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>38.5030483195589</v>
-      </c>
-      <c r="C3">
-        <v>0.932003922286742</v>
-      </c>
-      <c r="D3">
-        <v>65.851720274116502</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>37.539889448001098</v>
-      </c>
-      <c r="C4">
-        <v>0.95160008149895203</v>
-      </c>
-      <c r="D4">
-        <v>66.349948798948205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>36.134009305720198</v>
-      </c>
-      <c r="C5">
-        <v>0.94131340610499803</v>
-      </c>
-      <c r="D5">
-        <v>65.132674958110002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>36.039526794667097</v>
-      </c>
-      <c r="C6">
-        <v>0.96036726894812197</v>
-      </c>
-      <c r="D6">
-        <v>66.038126844739693</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>33.928665091189501</v>
-      </c>
-      <c r="C7">
-        <v>0.91442931109096803</v>
-      </c>
-      <c r="D7">
-        <v>62.685798100143103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>33.179587622441097</v>
-      </c>
-      <c r="C8">
-        <v>0.92489999698626202</v>
-      </c>
-      <c r="D8">
-        <v>62.834793660533698</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>32.455429447954998</v>
-      </c>
-      <c r="C9">
-        <v>0.87684136532493395</v>
-      </c>
-      <c r="D9">
-        <v>60.069782990224198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>33.134968365737102</v>
-      </c>
-      <c r="C10">
-        <v>0.92512203188226805</v>
-      </c>
-      <c r="D10">
-        <v>62.823585776982</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
         <v>3</v>
-      </c>
-      <c r="B11">
-        <v>33.0925733127008</v>
-      </c>
-      <c r="C11">
-        <v>0.91010291771046403</v>
-      </c>
-      <c r="D11">
-        <v>62.051432541873602</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>31.337176118089499</v>
-      </c>
-      <c r="C12">
-        <v>0.82165985494790605</v>
-      </c>
-      <c r="D12">
-        <v>56.751580806440003</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>